<commit_message>
1. Upgraded Django from 4.x to 5.2.6. 2. Refactored some code. 3. Applied some bug fixes.
</commit_message>
<xml_diff>
--- a/apps/es/resources/screen/ES001B.xlsx
+++ b/apps/es/resources/screen/ES001B.xlsx
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:T61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="C10" s="11" t="inlineStr">
         <is>
-          <t>es.views.es001b_views.ES001B</t>
+          <t>es.views.es001.ES001B</t>
         </is>
       </c>
       <c r="D10" s="8" t="n"/>
@@ -1325,7 +1325,7 @@
         </is>
       </c>
       <c r="C14" s="11" t="n">
-        <v>20250214135416</v>
+        <v>20250902100600</v>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
@@ -1447,6 +1447,7 @@
       <c r="I19" s="11" t="n"/>
     </row>
     <row r="20">
+      <c r="A20" s="6" t="n"/>
       <c r="C20" s="11" t="inlineStr">
         <is>
           <t>payeeRcs</t>
@@ -1468,6 +1469,7 @@
       <c r="I20" s="11" t="n"/>
     </row>
     <row r="21">
+      <c r="A21" s="6" t="n"/>
       <c r="C21" s="11" t="inlineStr">
         <is>
           <t>schRc</t>
@@ -1706,6 +1708,7 @@
       <c r="T27" s="11" t="n"/>
     </row>
     <row r="28">
+      <c r="B28" s="1" t="n"/>
       <c r="C28" s="11" t="inlineStr">
         <is>
           <t>payeeFg</t>
@@ -1764,6 +1767,7 @@
       <c r="T28" s="11" t="n"/>
     </row>
     <row r="29">
+      <c r="B29" s="1" t="n"/>
       <c r="C29" s="11" t="inlineStr">
         <is>
           <t>actionBar</t>
@@ -1981,6 +1985,7 @@
       <c r="P35" s="11" t="n"/>
     </row>
     <row r="36">
+      <c r="B36" s="1" t="n"/>
       <c r="C36" s="11" t="n"/>
       <c r="D36" s="11" t="inlineStr">
         <is>
@@ -2009,6 +2014,7 @@
       <c r="P36" s="11" t="n"/>
     </row>
     <row r="37">
+      <c r="B37" s="1" t="n"/>
       <c r="C37" s="11" t="inlineStr">
         <is>
           <t>payeeFg</t>
@@ -2024,7 +2030,11 @@
       <c r="G37" s="11" t="n"/>
       <c r="H37" s="11" t="n"/>
       <c r="I37" s="11" t="n"/>
-      <c r="J37" s="11" t="n"/>
+      <c r="J37" s="11" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="K37" s="11" t="inlineStr">
         <is>
           <t>ComboBox</t>
@@ -2046,6 +2056,7 @@
       <c r="P37" s="11" t="n"/>
     </row>
     <row r="38">
+      <c r="B38" s="1" t="n"/>
       <c r="C38" s="11" t="n"/>
       <c r="D38" s="11" t="n"/>
       <c r="E38" s="11" t="inlineStr">
@@ -2074,6 +2085,7 @@
       <c r="P38" s="11" t="n"/>
     </row>
     <row r="39">
+      <c r="B39" s="1" t="n"/>
       <c r="C39" s="11" t="n"/>
       <c r="D39" s="11" t="n"/>
       <c r="E39" s="11" t="inlineStr">
@@ -2102,6 +2114,7 @@
       <c r="P39" s="11" t="n"/>
     </row>
     <row r="40">
+      <c r="B40" s="1" t="n"/>
       <c r="C40" s="11" t="n"/>
       <c r="D40" s="11" t="n"/>
       <c r="E40" s="11" t="inlineStr">
@@ -2130,6 +2143,7 @@
       <c r="P40" s="11" t="n"/>
     </row>
     <row r="41">
+      <c r="B41" s="1" t="n"/>
       <c r="C41" s="11" t="inlineStr">
         <is>
           <t>actionBar</t>

</xml_diff>